<commit_message>
Commit all the differences
</commit_message>
<xml_diff>
--- a/Additional_files/Excel_with_values.xlsx
+++ b/Additional_files/Excel_with_values.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\University of Technology Delft\Master\MSc 1\Q1 AE4301 Automatic Flight Control System Design\Assignment\AFCSD_F16_Fighting_Falcon\Additional_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61FB6591-C5D1-455D-AFD0-FFB16D7294D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4852F359-0AB2-4CA3-943B-D4226C463570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86F6CCC3-E1F3-4CF2-8780-0CAF8EB18033}"/>
+    <workbookView xWindow="1164" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{86F6CCC3-E1F3-4CF2-8780-0CAF8EB18033}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,12 +34,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>delta_t</t>
+  </si>
+  <si>
+    <t>delta_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v </t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta_t </t>
+  </si>
+  <si>
+    <t>Orginal</t>
+  </si>
+  <si>
+    <t>Rows changed</t>
+  </si>
+  <si>
+    <t>Columns changed</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,13 +85,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,9 +120,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,180 +444,786 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D5BBB-6B8C-447B-8CCF-3A80FB5E8B8F}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
     <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>599.99999998824103</v>
       </c>
-      <c r="C1" s="1">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1">
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
         <v>-599.99999998824103</v>
       </c>
-      <c r="E1" s="1">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>1.2500603402246401E-4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>-32.169999999369999</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>-1.12975975340003E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>5.3132538741018198</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>-1.1274854857910399</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>1.5629034092777101E-3</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <v>5.1447106153613802E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>-32.169999999369999</v>
+      </c>
+      <c r="L3">
+        <v>-1.12975975340003E-2</v>
+      </c>
+      <c r="M3">
+        <v>5.3132538741018198</v>
+      </c>
+      <c r="N3">
+        <v>-1.1274854857910399</v>
+      </c>
+      <c r="P3">
+        <v>5.1447106153613802E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.9576455750341701E-6</v>
       </c>
       <c r="B4" s="1">
         <v>7.6495756674730601E-14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>-1.7692499402202001E-4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>-0.457651811188105</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>0.96271539873711098</v>
       </c>
       <c r="F4" s="1">
         <v>-2.48627558449417E-7</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>-9.6997977157705598E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1">
+        <v>7.6495756674730601E-14</v>
+      </c>
+      <c r="L4">
+        <v>-1.7692499402202001E-4</v>
+      </c>
+      <c r="M4">
+        <v>-0.457651811188105</v>
+      </c>
+      <c r="N4">
+        <v>0.96271539873711098</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4">
+        <v>-9.6997977157705598E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>-1.87425213086328E-20</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>1.6938819327552E-18</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>-1.8486746274657999</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>-0.63612645690444702</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>-9.7361214892929093E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="J5" s="1"/>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.6938819327552E-18</v>
+      </c>
+      <c r="M5">
+        <v>-1.8486746274657999</v>
+      </c>
+      <c r="N5">
+        <v>-0.63612645690444702</v>
+      </c>
+      <c r="P5">
+        <v>-9.7361214892929093E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>-1</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>-20.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>-20.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9E8C1B-CF0F-402D-96A6-A93B5CD6819F}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>-32.169999999369999</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-1.12975975340003E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.3132538741018198</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-1.1274854857910399</v>
+      </c>
+      <c r="E4">
+        <v>1.5629034092777101E-3</v>
+      </c>
+      <c r="F4">
+        <v>5.1447106153613802E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>7.6495756674730601E-14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-1.7692499402202001E-4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-0.457651811188105</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.96271539873711098</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-2.48627558449417E-7</v>
+      </c>
+      <c r="F5">
+        <v>-9.6997977157705598E-4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.6938819327552E-18</v>
+      </c>
+      <c r="C6">
+        <v>-1.8486746274657999</v>
+      </c>
+      <c r="D6">
+        <v>-0.63612645690444702</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>-9.7361214892929093E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>-20.2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>-32.169999999369999</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-1.12975975340003E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.3132538741018198</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-1.1274854857910399</v>
+      </c>
+      <c r="E12">
+        <v>1.5629034092777101E-3</v>
+      </c>
+      <c r="F12">
+        <v>5.1447106153613802E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>7.6495756674730601E-14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-1.7692499402202001E-4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-0.457651811188105</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.96271539873711098</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-2.48627558449417E-7</v>
+      </c>
+      <c r="F13">
+        <v>-9.6997977157705598E-4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.6938819327552E-18</v>
+      </c>
+      <c r="C15">
+        <v>-1.8486746274657999</v>
+      </c>
+      <c r="D15">
+        <v>-0.63612645690444702</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>-9.7361214892929093E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>-20.2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>-1.12975975340003E-2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5.3132538741018198</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-32.169999999369999</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-1.1274854857910399</v>
+      </c>
+      <c r="E21">
+        <v>5.1447106153613802E-2</v>
+      </c>
+      <c r="F21">
+        <v>1.5629034092777101E-3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>-1.7692499402202001E-4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>-0.457651811188105</v>
+      </c>
+      <c r="C22" s="2">
+        <v>7.6495756674730601E-14</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.96271539873711098</v>
+      </c>
+      <c r="E22">
+        <v>-9.6997977157705598E-4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-2.48627558449417E-7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1.6938819327552E-18</v>
+      </c>
+      <c r="B24">
+        <v>-1.8486746274657999</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>-0.63612645690444702</v>
+      </c>
+      <c r="E24">
+        <v>-9.7361214892929093E-2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>-20.2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>